<commit_message>
rust byor ui data
</commit_message>
<xml_diff>
--- a/_data/technology-list.xlsx
+++ b/_data/technology-list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JulianDariel/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="575" documentId="8_{78B5569B-D514-0945-B667-FE1EFE27097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{612DC173-8CD0-47AF-A83C-A7E165146F05}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96100BBD-50D1-490C-BD6E-6F961D441A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{2F4ADB98-FD6B-8342-A7E2-5A959F028097}"/>
   </bookViews>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="104">
   <si>
     <t>Technology</t>
   </si>
@@ -145,27 +146,36 @@
     <t>Node.JS</t>
   </si>
   <si>
+    <t xml:space="preserve">Node.js® is a JavaScript runtime built on Chrome's V8 JavaScript engine. JS on the backend. </t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Rust</t>
+  </si>
+  <si>
     <t>Adopt</t>
   </si>
   <si>
-    <t xml:space="preserve">"Node.js® is a JavaScript runtime built on Chrome's V8 JavaScript engine." JS on the backend. </t>
-  </si>
-  <si>
-    <t>Limited</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Rust</t>
-  </si>
-  <si>
-    <t>"Rust is blazingly fast and memory-efficient: with no runtime or garbage collector, it can power performance-critical services, run on embedded devices, and easily integrate with other languages."</t>
+    <t>Rust is blazingly fast and memory-efficient: with no runtime or garbage collector, it can power performance-critical services, run on embedded devices, and easily integrate with other languages</t>
   </si>
   <si>
     <t>Mozilla</t>
   </si>
   <si>
+    <t>Q3 - 2022</t>
+  </si>
+  <si>
+    <t>mature enough to be used in micro-service architectures for web API micro service deployments as container orchestrated pods in k8s or serverless eg AWS lambda functions where processing performance and memory management are critical</t>
+  </si>
+  <si>
     <t>Cloud RPA</t>
   </si>
   <si>
@@ -233,9 +243,6 @@
   </si>
   <si>
     <t>Helps develop web applications that work as well offline as they do online. PouchDB is an open-source JavaScript database inspired by Apache CouchDB and designed to run within the browser.</t>
-  </si>
-  <si>
-    <t>Q3 - 2022</t>
   </si>
   <si>
     <t>enables applications to store data locally while offline, then synchronize it with CouchDB and compatible servers when the application is back online, keeping the user's data in sync no matter where they next login</t>
@@ -444,7 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -475,9 +482,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -812,8 +818,8 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="E2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" customHeight="1"/>
@@ -952,7 +958,7 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -961,6 +967,9 @@
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
         <v>31</v>
       </c>
       <c r="I5" t="s">
@@ -975,7 +984,7 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -984,38 +993,50 @@
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="18.75" customHeight="1">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="18.75" customHeight="1">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1027,10 +1048,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
@@ -1041,7 +1062,7 @@
     </row>
     <row r="9" spans="1:11" ht="18.75" customHeight="1">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1053,10 +1074,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>
@@ -1064,7 +1085,7 @@
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>12</v>
@@ -1076,27 +1097,27 @@
         <v>0</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>25</v>
@@ -1108,13 +1129,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>32</v>
@@ -1125,7 +1146,7 @@
     </row>
     <row r="12" spans="1:11" ht="18.75" customHeight="1">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -1137,15 +1158,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>12</v>
@@ -1157,53 +1178,53 @@
         <v>0</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="17" customFormat="1" ht="18.75" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" customHeight="1">
       <c r="A14" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>63</v>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>13</v>
@@ -1212,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>22</v>
@@ -1230,12 +1251,12 @@
         <v>33</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -1247,32 +1268,32 @@
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" t="s">
         <v>72</v>
-      </c>
-      <c r="K16" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="18.75" customHeight="1">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="18.75" customHeight="1">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
@@ -1284,15 +1305,15 @@
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>12</v>
@@ -1304,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>15</v>
@@ -1313,7 +1334,7 @@
         <v>22</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>18</v>
@@ -1322,7 +1343,7 @@
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>12</v>
@@ -1334,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>21</v>
@@ -1354,7 +1375,7 @@
     </row>
     <row r="21" spans="1:11" ht="18.75" customHeight="1">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -1366,18 +1387,18 @@
         <v>0</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="18.75" customHeight="1">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -1385,37 +1406,37 @@
     </row>
     <row r="23" spans="1:11" ht="18.75" customHeight="1">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:11" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D24" s="9" t="b">
         <v>0</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>15</v>
@@ -1424,10 +1445,10 @@
         <v>22</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>33</v>
@@ -1435,64 +1456,64 @@
     </row>
     <row r="25" spans="1:11" ht="18.75" customHeight="1">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" customHeight="1">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D27" s="9" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>22</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>33</v>
@@ -1500,7 +1521,7 @@
     </row>
     <row r="28" spans="1:11" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>12</v>
@@ -1512,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>15</v>
@@ -1521,24 +1542,24 @@
         <v>22</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A29" s="13" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D29" s="9" t="b">
         <v>0</v>
@@ -1551,10 +1572,10 @@
         <v>22</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J29" s="9" t="s">
         <v>33</v>
@@ -1581,12 +1602,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B35205D5F59A4D4BBCA883FBC2FA3943" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b15e43a1c96e46df86d2e1e839c839a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="837ce9e9-8e91-45ed-b36e-9f6e76e50cf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="617d7c17d802374d700bc0b6aca7e1bc" ns2:_="">
     <xsd:import namespace="837ce9e9-8e91-45ed-b36e-9f6e76e50cf3"/>
@@ -1750,14 +1765,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02926F97-9605-4A94-8210-FF513A9089FB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{641B8296-0A07-4A1A-9684-52CE07BE4B9B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{942D78DD-FC5B-4C29-B184-2C861DD1BDD8}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{942D78DD-FC5B-4C29-B184-2C861DD1BDD8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{641B8296-0A07-4A1A-9684-52CE07BE4B9B}"/>
 </file>
</xml_diff>